<commit_message>
AVANCES REPORTE GENERAL ALTAS
</commit_message>
<xml_diff>
--- a/WebAppSISGEFIN/Templates/Patrimonio/Template_InventarioInicial.xlsx
+++ b/WebAppSISGEFIN/Templates/Patrimonio/Template_InventarioInicial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\IAFAS\IAFAS\WebAppSISGEFIN\Templates\Patrimonio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95520766-7B04-4183-A9D7-C201B1663929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB010C9-3283-4531-B596-3CC988735311}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C817FBA-B522-48F5-BDF1-5C32D75E90BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="93">
   <si>
     <t>NRO_DOCUMENTO_NEA</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>MEDIDAS</t>
-  </si>
-  <si>
-    <t>SUB_CTA</t>
   </si>
   <si>
     <t>MAYOR</t>
@@ -1305,6 +1302,30 @@
   </si>
   <si>
     <t>2.6.32.31</t>
+  </si>
+  <si>
+    <t>020301</t>
+  </si>
+  <si>
+    <t>7408995001010</t>
+  </si>
+  <si>
+    <t>7408995001011</t>
+  </si>
+  <si>
+    <t>740880370005</t>
+  </si>
+  <si>
+    <t>7408803701008</t>
+  </si>
+  <si>
+    <t>MONITOR LED 21.5 in</t>
+  </si>
+  <si>
+    <t>2500.00000</t>
+  </si>
+  <si>
+    <t>7408803701009</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1486,15 +1507,6 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1510,9 +1522,6 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1552,8 +1561,33 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1880,17 +1914,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF681B9-E44D-47AF-A5DD-5C17DCDE0969}">
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="24" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="24" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
@@ -1898,323 +1932,714 @@
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="22" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="22" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="16" max="16" width="23" customWidth="1"/>
-    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="27" style="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" style="22" customWidth="1"/>
     <col min="19" max="19" width="28.5703125" customWidth="1"/>
     <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.5703125" customWidth="1"/>
     <col min="22" max="22" width="13.7109375" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="22" customWidth="1"/>
     <col min="24" max="24" width="27.42578125" customWidth="1"/>
     <col min="25" max="25" width="19.140625" customWidth="1"/>
-    <col min="26" max="26" width="21.7109375" customWidth="1"/>
+    <col min="26" max="26" width="21.7109375" style="22" customWidth="1"/>
     <col min="27" max="27" width="17.7109375" customWidth="1"/>
     <col min="28" max="29" width="20.140625" customWidth="1"/>
     <col min="30" max="30" width="18.7109375" customWidth="1"/>
+    <col min="31" max="32" width="11.42578125" style="22"/>
     <col min="33" max="33" width="19.85546875" customWidth="1"/>
     <col min="34" max="34" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="180" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="Q1" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z1" s="6" t="s">
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AD2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AC2" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE2" s="13" t="s">
+      <c r="AE2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AF2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH2" s="14" t="s">
-        <v>25</v>
+      <c r="AH2" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19">
+        <v>2</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="20">
+        <v>44691</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="20">
+        <v>44693</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="AD3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE3" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF3" s="17">
+        <v>1503</v>
+      </c>
+      <c r="AG3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH3" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19">
+        <v>2</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="L4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="20">
+        <v>44691</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="20">
+        <v>44693</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC4" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE4" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF4" s="17">
+        <v>1503</v>
+      </c>
+      <c r="AG4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH4" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="21" t="s">
+      <c r="E5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19">
+        <v>2</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="20">
+        <v>44691</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="20">
+        <v>44693</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="23">
+      <c r="AE5" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF5" s="17">
+        <v>1503</v>
+      </c>
+      <c r="AG5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH5" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="G3" s="23">
+      <c r="C6" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="29">
+        <v>1</v>
+      </c>
+      <c r="G6" s="29">
         <v>2</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="21" t="s">
+      <c r="K6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" s="20">
+        <v>44691</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="20">
+        <v>44693</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="24">
+      <c r="U6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="W6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="X6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF6" s="17">
+        <v>1503</v>
+      </c>
+      <c r="AG6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH6" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <v>1</v>
+      </c>
+      <c r="G7" s="29">
+        <v>2</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" s="20">
         <v>44691</v>
       </c>
-      <c r="N3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="24">
+      <c r="N7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="20">
         <v>44693</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="21" t="s">
+      <c r="P7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="W3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="X3" s="21" t="s">
+      <c r="AA7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Y3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z3" s="21" t="s">
+      <c r="AB7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF7" s="17">
+        <v>1503</v>
+      </c>
+      <c r="AG7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH7" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="AA3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC3" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH3" s="21" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>